<commit_message>
Upload Y3_B2526_GIT_&_Liver_schedule.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/modules_schedules/Y3_B2526_GIT_&_Liver_schedule.xlsx
+++ b/modules_schedules/Y3_B2526_GIT_&_Liver_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\modules_schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53455A25-0F3E-4AA8-B7E3-69E007CF1791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E968B10-7BA7-4D79-B706-8F26EF09BC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="60">
   <si>
     <t>Year</t>
   </si>
@@ -685,8 +685,8 @@
       <c r="D4" s="2">
         <v>3</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>12</v>
+      <c r="E4" s="3">
+        <v>45945</v>
       </c>
       <c r="F4" s="4">
         <v>0.58333333333333337</v>
@@ -896,7 +896,7 @@
         <v>18</v>
       </c>
       <c r="F13" s="8">
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="G13" s="9">
         <v>120</v>
@@ -1241,7 +1241,7 @@
         <v>20</v>
       </c>
       <c r="F28" s="4">
-        <v>8.3333333333333329E-2</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G28" s="5">
         <v>120</v>
@@ -2640,8 +2640,8 @@
       <c r="D89" s="6">
         <v>1</v>
       </c>
-      <c r="E89" s="7" t="s">
-        <v>22</v>
+      <c r="E89" s="7">
+        <v>45938</v>
       </c>
       <c r="F89" s="8">
         <v>0.5</v>
@@ -2663,11 +2663,11 @@
       <c r="D90" s="2">
         <v>2</v>
       </c>
-      <c r="E90" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F90" s="4">
-        <v>0.5</v>
+      <c r="E90" s="3">
+        <v>45958</v>
+      </c>
+      <c r="F90" s="8">
+        <v>0.41666666666666669</v>
       </c>
       <c r="G90" s="5">
         <v>120</v>
@@ -2686,11 +2686,11 @@
       <c r="D91" s="6">
         <v>1</v>
       </c>
-      <c r="E91" s="7" t="s">
-        <v>45</v>
+      <c r="E91" s="7">
+        <v>45929</v>
       </c>
       <c r="F91" s="8">
-        <v>0.41666666666666669</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G91" s="9">
         <v>75</v>
@@ -3380,7 +3380,7 @@
         <v>53</v>
       </c>
       <c r="F121" s="8">
-        <v>8.3333333333333329E-2</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="G121" s="9">
         <v>120</v>
@@ -3745,7 +3745,7 @@
         <v>2</v>
       </c>
       <c r="E137" s="7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F137" s="8">
         <v>0.58333333333333337</v>
@@ -4641,11 +4641,11 @@
       <c r="D176" s="2">
         <v>1</v>
       </c>
-      <c r="E176" s="3" t="s">
-        <v>16</v>
+      <c r="E176" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="F176" s="4">
-        <v>0.58333333333333337</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G176" s="5">
         <v>75</v>
@@ -4848,11 +4848,11 @@
       <c r="D185" s="6">
         <v>2</v>
       </c>
-      <c r="E185" s="7" t="s">
-        <v>39</v>
+      <c r="E185" s="7">
+        <v>45943</v>
       </c>
       <c r="F185" s="8">
-        <v>0.45833333333333331</v>
+        <v>0.375</v>
       </c>
       <c r="G185" s="9">
         <v>75</v>
@@ -4905,6 +4905,12 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G187">
+    <sortCondition ref="B2:B187"/>
+    <sortCondition ref="C2:C187"/>
+    <sortCondition ref="D2:D187"/>
+    <sortCondition ref="E2:E187"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>